<commit_message>
Update Reports and Add Huabao power alert
</commit_message>
<xml_diff>
--- a/templates/export/events.xlsx
+++ b/templates/export/events.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27880" windowHeight="16760" tabRatio="989"/>
+    <workbookView xWindow="4080" yWindow="-21140" windowWidth="19780" windowHeight="16760" tabRatio="989"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
             <family val="2"/>
             <charset val="204"/>
           </rPr>
-          <t>jx:area(lastCell="E9")</t>
+          <t>jx:area(lastCell="D24")</t>
         </r>
       </text>
     </comment>
@@ -59,11 +59,11 @@
             <family val="2"/>
             <charset val="204"/>
           </rPr>
-          <t>jx:each(items="devices", var="device", lastCell="E9" multisheet="sheetNames")</t>
+          <t>jx:each(items="devices", var="device", lastCell="D24" multisheet="sheetNames")</t>
         </r>
       </text>
     </comment>
-    <comment ref="A9" authorId="0">
+    <comment ref="A23" authorId="0">
       <text>
         <r>
           <rPr>
@@ -73,7 +73,7 @@
             <family val="2"/>
             <charset val="204"/>
           </rPr>
-          <t>jx:each(items="device.objects", var="event", lastCell="B9")</t>
+          <t>jx:each(items="device.objects", var="event", lastCell="D24")</t>
         </r>
       </text>
     </comment>
@@ -82,20 +82,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t>Report type:</t>
-  </si>
-  <si>
-    <t>Events</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="52">
   <si>
     <t>Device:</t>
   </si>
   <si>
-    <t>${device.deviceName}</t>
-  </si>
-  <si>
     <t>Group:</t>
   </si>
   <si>
@@ -105,19 +96,148 @@
     <t>Period:</t>
   </si>
   <si>
-    <t>${dateTool.format("YYYY-MM-dd HH:mm:ss", from, locale, timezone)+" - "+dateTool.format("YYYY-MM-dd HH:mm:ss", to, locale, timezone)}</t>
-  </si>
-  <si>
-    <t>Time</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
     <t>${dateTool.format("YYYY-MM-dd HH:mm:ss", event.serverTime, locale, timezone)}</t>
   </si>
   <si>
     <t>${event.typeForExcel}</t>
+  </si>
+  <si>
+    <t>የባለቤቱ ስም</t>
+  </si>
+  <si>
+    <t>ፆታ</t>
+  </si>
+  <si>
+    <t>Contact</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>ሞዴል</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>የተሰራበት ሀገር</t>
+  </si>
+  <si>
+    <t>Country of Manuf</t>
+  </si>
+  <si>
+    <t>የሞተር ቁጥር</t>
+  </si>
+  <si>
+    <t>Engine Number</t>
+  </si>
+  <si>
+    <t>የGPS ሞዴል</t>
+  </si>
+  <si>
+    <t>GPS Model</t>
+  </si>
+  <si>
+    <t>የሲም ካርድ ቁጥር</t>
+  </si>
+  <si>
+    <t>SIM Number</t>
+  </si>
+  <si>
+    <t>ታርጋ ቁጥር</t>
+  </si>
+  <si>
+    <t>Plate Number</t>
+  </si>
+  <si>
+    <t>የተሰራበት ዓ/ምህረት</t>
+  </si>
+  <si>
+    <t>Manuf Year</t>
+  </si>
+  <si>
+    <t>ሻንሲ ቁጥር</t>
+  </si>
+  <si>
+    <t>Chassis Number</t>
+  </si>
+  <si>
+    <t>IMEI ቁጥር</t>
+  </si>
+  <si>
+    <t>IMEI Number</t>
+  </si>
+  <si>
+    <t>የሲም ካርድ  ICCID ቁጥር</t>
+  </si>
+  <si>
+    <t>SIM ICCID Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">የመቆጣተሪያ ሲስተም </t>
+  </si>
+  <si>
+    <t>Web Site</t>
+  </si>
+  <si>
+    <t>የተመዘገበበት  ቀን</t>
+  </si>
+  <si>
+    <t>Membership Date</t>
+  </si>
+  <si>
+    <t>monitor.ethiogps.com</t>
+  </si>
+  <si>
+    <t>${device.device.contact}</t>
+  </si>
+  <si>
+    <t>${device.device.vehicleModel}</t>
+  </si>
+  <si>
+    <t>${device.device.countryOfManufacturing}</t>
+  </si>
+  <si>
+    <t>${device.device.engineNumber}</t>
+  </si>
+  <si>
+    <t>${device.device.model}</t>
+  </si>
+  <si>
+    <t>${device.device.simNumber}</t>
+  </si>
+  <si>
+    <t>${device.device.gender}</t>
+  </si>
+  <si>
+    <t>${device.device.plateNumber}</t>
+  </si>
+  <si>
+    <t>${device.device.chassisNumber}</t>
+  </si>
+  <si>
+    <t>${device.device.manufacturingYear}</t>
+  </si>
+  <si>
+    <t>${device.device.uniqueId}</t>
+  </si>
+  <si>
+    <t>${device.device.simIccidNumber}</t>
+  </si>
+  <si>
+    <t>${dateTool.format("YYYY-MM-dd", from, locale, timezone)+" - "+dateTool.format("YYYY-MM-dd", to, locale, timezone)}</t>
+  </si>
+  <si>
+    <t>${dateTool.format("YYYY-MM-dd", device.device.membershipDate, locale, timezone)}</t>
+  </si>
+  <si>
+    <t>Device Event Report</t>
+  </si>
+  <si>
+    <t>Event Time</t>
+  </si>
+  <si>
+    <t>Event Type</t>
   </si>
 </sst>
 </file>
@@ -127,7 +247,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -144,52 +264,139 @@
       <charset val="204"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FF444444"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Abyssinica SIL"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF444444"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Abyssinica SIL"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="204"/>
-    </font>
-    <font>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF444444"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="10"/>
       <color rgb="FF444444"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF333333"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-      <charset val="204"/>
+      <color theme="8" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="24"/>
+      <color rgb="FF444444"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="24"/>
+      <color rgb="FF444444"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -202,8 +409,19 @@
         <bgColor rgb="FF969696"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -226,41 +444,136 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="15"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="15"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -354,10 +667,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>3368540</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1984240</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>171360</xdr:rowOff>
+      <xdr:rowOff>31660</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -405,10 +718,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>3368540</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1984240</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>171360</xdr:rowOff>
+      <xdr:rowOff>31660</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -456,10 +769,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>3368540</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1984240</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>171360</xdr:rowOff>
+      <xdr:rowOff>31660</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -507,9 +820,9 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>62</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -550,9 +863,9 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>62</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -593,9 +906,9 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>62</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -894,80 +1207,291 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="57.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="108.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.1640625" customWidth="1"/>
+    <col min="2" max="2" width="33.6640625" customWidth="1"/>
+    <col min="3" max="3" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+    </row>
+    <row r="3" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B3" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="11"/>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="1"/>
-      <c r="B3" s="3"/>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="B4" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="C4" s="11"/>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+      <c r="B5" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="11"/>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="13"/>
+      <c r="C8" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="16"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="14"/>
+      <c r="C10" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="16"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="15"/>
+      <c r="C12" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="16"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="15"/>
+      <c r="C14" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="16"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="15"/>
+      <c r="C16" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="16"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="15"/>
+      <c r="C18" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" s="16"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="20"/>
+      <c r="C20" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" s="18"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+    </row>
+    <row r="22" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B22" s="4"/>
+      <c r="C22" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D22" s="4"/>
+    </row>
+    <row r="23" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B23" s="6"/>
+      <c r="C23" s="7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="5"/>
-      <c r="B7" s="6"/>
-    </row>
-    <row r="8" spans="1:2" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>11</v>
-      </c>
+      <c r="D23" s="8"/>
     </row>
   </sheetData>
-  <pageMargins left="0.70833333333333304" right="0.70833333333333304" top="0.74791666666666701" bottom="0.74791666666666701" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
+  <mergeCells count="22">
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="B17:B18"/>
+  </mergeCells>
+  <phoneticPr fontId="11" type="noConversion"/>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.71" right="0.71" top="0.25" bottom="0.25" header="0.26" footer="0.26"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Event Alert disconnected and low battery to be one
</commit_message>
<xml_diff>
--- a/templates/export/events.xlsx
+++ b/templates/export/events.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4080" yWindow="-21140" windowWidth="19780" windowHeight="16760" tabRatio="989"/>
+    <workbookView xWindow="4320" yWindow="-21140" windowWidth="22760" windowHeight="16760" tabRatio="989"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="1" r:id="rId1"/>
@@ -39,13 +39,13 @@
       <text>
         <r>
           <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
-            <charset val="204"/>
           </rPr>
-          <t>jx:area(lastCell="D24")</t>
+          <t>jx:area(lastCell="E22")</t>
         </r>
       </text>
     </comment>
@@ -53,27 +53,27 @@
       <text>
         <r>
           <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
-            <charset val="204"/>
           </rPr>
-          <t>jx:each(items="devices", var="device", lastCell="D24" multisheet="sheetNames")</t>
+          <t>jx:each(items="devices", var="device", lastCell="E22" multisheet="sheetNames")</t>
         </r>
       </text>
     </comment>
-    <comment ref="A23" authorId="0">
+    <comment ref="A22" authorId="0">
       <text>
         <r>
           <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
-            <charset val="204"/>
           </rPr>
-          <t>jx:each(items="device.objects", var="event", lastCell="D24")</t>
+          <t>jx:each(items="device.objects", var="event", lastCell="E22")</t>
         </r>
       </text>
     </comment>
@@ -82,19 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="52">
-  <si>
-    <t>Device:</t>
-  </si>
-  <si>
-    <t>Group:</t>
-  </si>
-  <si>
-    <t>${device.groupName}</t>
-  </si>
-  <si>
-    <t>Period:</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>${dateTool.format("YYYY-MM-dd HH:mm:ss", event.serverTime, locale, timezone)}</t>
   </si>
@@ -225,9 +213,6 @@
     <t>${device.device.simIccidNumber}</t>
   </si>
   <si>
-    <t>${dateTool.format("YYYY-MM-dd", from, locale, timezone)+" - "+dateTool.format("YYYY-MM-dd", to, locale, timezone)}</t>
-  </si>
-  <si>
     <t>${dateTool.format("YYYY-MM-dd", device.device.membershipDate, locale, timezone)}</t>
   </si>
   <si>
@@ -238,6 +223,15 @@
   </si>
   <si>
     <t>Event Type</t>
+  </si>
+  <si>
+    <t>Device: ${device.device.contact}</t>
+  </si>
+  <si>
+    <t>Group: ${device.groupName}</t>
+  </si>
+  <si>
+    <t>Period: ${dateTool.format("YYYY-MM-dd", from, locale, timezone)+" - "+dateTool.format("YYYY-MM-dd", to, locale, timezone)}</t>
   </si>
 </sst>
 </file>
@@ -247,7 +241,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -292,13 +286,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-      <charset val="204"/>
     </font>
     <font>
       <sz val="12"/>
@@ -316,14 +303,6 @@
     <font>
       <b/>
       <sz val="14"/>
-      <color rgb="FF444444"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -392,6 +371,13 @@
       <b/>
       <sz val="24"/>
       <color rgb="FF444444"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color indexed="81"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -421,7 +407,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -436,19 +422,6 @@
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
       <top style="thin">
         <color auto="1"/>
       </top>
@@ -500,9 +473,9 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -510,65 +483,53 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="15"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -667,10 +628,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1984240</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>31660</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>282440</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>107860</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -718,10 +679,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1984240</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>31660</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>282440</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>107860</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -769,10 +730,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1984240</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>31660</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>282440</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>107860</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -822,8 +783,8 @@
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>62</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -865,8 +826,8 @@
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>62</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -908,8 +869,8 @@
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>62</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1207,18 +1168,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.1640625" customWidth="1"/>
-    <col min="2" max="2" width="33.6640625" customWidth="1"/>
-    <col min="3" max="3" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34" customWidth="1"/>
+    <col min="1" max="1" width="20.1640625" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" customWidth="1"/>
+    <col min="3" max="3" width="21.1640625" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1228,270 +1189,257 @@
       <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+    </row>
+    <row r="3" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" s="8"/>
+    </row>
+    <row r="4" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-    </row>
-    <row r="3" spans="1:4" ht="19" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="12"/>
+      <c r="C7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="7"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="13"/>
+      <c r="C9" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="7"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="14"/>
+      <c r="C11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="7"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="14"/>
+      <c r="C13" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="7"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="14"/>
+      <c r="C15" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="7"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="14"/>
+      <c r="C17" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" s="7"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="16"/>
+      <c r="C19" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" s="18"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" s="9"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:4" ht="19" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="B22" s="10"/>
+      <c r="C22" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:4" ht="19" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="C5" s="11"/>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="16" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="16"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="14"/>
-      <c r="C10" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="16"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="16" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="15"/>
-      <c r="C12" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="16"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="15"/>
-      <c r="C14" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14" s="16"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15" s="16" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="15"/>
-      <c r="C16" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="D16" s="16"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D17" s="16" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" s="15"/>
-      <c r="C18" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="D18" s="16"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B19" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="D19" s="17" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="B20" s="20"/>
-      <c r="C20" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D20" s="18"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-    </row>
-    <row r="22" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B22" s="4"/>
-      <c r="C22" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D22" s="4"/>
-    </row>
-    <row r="23" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B23" s="6"/>
-      <c r="C23" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D23" s="8"/>
+      <c r="D22" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="D16:D17"/>
     <mergeCell ref="A2:D2"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A3:B3"/>
   </mergeCells>
-  <phoneticPr fontId="11" type="noConversion"/>
-  <printOptions horizontalCentered="1"/>
-  <pageMargins left="0.71" right="0.71" top="0.25" bottom="0.25" header="0.26" footer="0.26"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="landscape" r:id="rId1"/>
+  <phoneticPr fontId="9" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.25" bottom="0.25" header="0.26" footer="0.26"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
 </worksheet>

</xml_diff>